<commit_message>
fix: Correction on alerts of view_add_atestado.py and save the changes did by view_rem_faltas on sheets
</commit_message>
<xml_diff>
--- a/planilhas/07-2025/6-07-2025.xlsx
+++ b/planilhas/07-2025/6-07-2025.xlsx
@@ -24,7 +24,7 @@
     <numFmt numFmtId="168" formatCode="dddd"/>
     <numFmt numFmtId="169" formatCode="#,##0;;&quot;-&quot;"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -163,8 +163,12 @@
       <b val="1"/>
       <color rgb="00FF0000"/>
     </font>
+    <font>
+      <b val="1"/>
+      <color rgb="000000FF"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill/>
     </fill>
@@ -213,6 +217,12 @@
         <bgColor rgb="00FFCCCC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00ADCBFF"/>
+        <bgColor rgb="00ADCBFF"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="50">
     <border>
@@ -838,7 +848,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
     <xf numFmtId="164" fontId="9" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
@@ -1227,6 +1237,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="167" fontId="19" fillId="8" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="20" fillId="9" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0" hidden="0"/>
     </xf>
@@ -4117,9 +4131,9 @@
         <f>WEEKDAY(B30)</f>
         <v/>
       </c>
-      <c r="D30" s="131" t="inlineStr">
-        <is>
-          <t>Falta sem Justificativa</t>
+      <c r="D30" s="132" t="inlineStr">
+        <is>
+          <t>Falta com Atestado</t>
         </is>
       </c>
       <c r="E30" s="117" t="n"/>
@@ -4720,8 +4734,8 @@
     <mergeCell ref="B2:S2"/>
     <mergeCell ref="Q4:S4"/>
     <mergeCell ref="Y4:AB4"/>
+    <mergeCell ref="D30:G30"/>
     <mergeCell ref="U4:V4"/>
-    <mergeCell ref="D30:G30"/>
     <mergeCell ref="I4:O4"/>
     <mergeCell ref="B39:D39"/>
     <mergeCell ref="E39:F39"/>

</xml_diff>